<commit_message>
preparando análisis con SonarQube y actualizando plantilla de calificación
</commit_message>
<xml_diff>
--- a/plantilla_experimento_3.xlsx
+++ b/plantilla_experimento_3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansanchez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansanchez/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Experimentación</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Desarrollo de la aplicación nativa Android o iOS del médico, desde esta debe poder hacer TODAS las funcionales que hace desde la Web. Una salvedad: de la historia clínica y de las medidas tomadas ve sólo la información más relevante.</t>
+  </si>
+  <si>
+    <t>Desarrollo de la aplicación nativa Android o iOS del paciente, desde esta debe poder hacer TODAS las funcionales presentes en el diagrama de casos de uso</t>
   </si>
   <si>
     <t>Correcciones de la interfaz Web con base en la realimentación de los usuarios de la crítica colaborativa. Se valorará el atractivo de la interfaz.</t>
@@ -92,6 +95,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -290,15 +296,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -328,12 +334,63 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1244600</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1244600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -635,11 +692,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y996"/>
+  <dimension ref="A1:Y997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18"/>
+      <selection pane="topRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -650,22 +707,22 @@
     <col min="13" max="21" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:25" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -681,18 +738,18 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+    <row r="2" spans="1:25" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -708,20 +765,20 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="19"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -742,9 +799,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -773,9 +832,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -804,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -830,20 +891,22 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
+      <c r="B7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -859,22 +922,20 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -891,13 +952,15 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -921,20 +984,22 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="B10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -950,22 +1015,20 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -981,20 +1044,22 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" ht="14" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="B12" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1010,22 +1075,20 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:25" ht="14" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1041,23 +1104,22 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:25" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9">
-        <f>SUM(B4:B13)</f>
-        <v>1</v>
+      <c r="B14" s="7">
+        <v>0.05</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1073,18 +1135,23 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+    <row r="15" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
+        <f>SUM(B4:B14)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1157,15 +1224,15 @@
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1181,18 +1248,18 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1208,18 +1275,18 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1262,7 +1329,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1"/>
@@ -1343,7 +1410,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="1"/>
@@ -1560,7 +1627,7 @@
       <c r="Y32" s="1"/>
     </row>
     <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="14"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1641,7 +1708,7 @@
       <c r="Y35" s="1"/>
     </row>
     <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="11"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="12"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1667,8 +1734,8 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
     </row>
-    <row r="37" spans="1:25" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="11"/>
       <c r="B37" s="12"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -27587,23 +27654,50 @@
       <c r="X996" s="1"/>
       <c r="Y996" s="1"/>
     </row>
+    <row r="997" spans="1:25" ht="13" x14ac:dyDescent="0.15">
+      <c r="A997" s="1"/>
+      <c r="B997" s="12"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="1"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="1"/>
+      <c r="G997" s="1"/>
+      <c r="H997" s="1"/>
+      <c r="I997" s="1"/>
+      <c r="J997" s="1"/>
+      <c r="K997" s="1"/>
+      <c r="L997" s="1"/>
+      <c r="M997" s="1"/>
+      <c r="N997" s="1"/>
+      <c r="O997" s="1"/>
+      <c r="P997" s="1"/>
+      <c r="Q997" s="1"/>
+      <c r="R997" s="1"/>
+      <c r="S997" s="1"/>
+      <c r="T997" s="1"/>
+      <c r="U997" s="1"/>
+      <c r="V997" s="1"/>
+      <c r="W997" s="1"/>
+      <c r="X997" s="1"/>
+      <c r="Y997" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>